<commit_message>
Testdata and helper changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0A205B-6493-4A1F-B678-938997621E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADBAB51-B7CD-47A5-9FD2-131BE130B95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28800" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="329">
   <si>
     <t>UserName</t>
   </si>
@@ -1019,6 +1019,9 @@
   </si>
   <si>
     <t>DRYQATEST20</t>
+  </si>
+  <si>
+    <t>vnarra@helenoftroy.com</t>
   </si>
 </sst>
 </file>
@@ -1446,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,7 +1610,9 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>328</v>
+      </c>
       <c r="C2" s="8"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1617,7 +1622,9 @@
       <c r="G2" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>328</v>
+      </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
@@ -1950,27 +1957,32 @@
       <c r="A19" t="s">
         <v>55</v>
       </c>
+      <c r="B19" t="s">
+        <v>328</v>
+      </c>
       <c r="F19" t="s">
         <v>47</v>
       </c>
       <c r="G19" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="8"/>
+      <c r="K19" s="8" t="s">
+        <v>328</v>
+      </c>
       <c r="N19" t="s">
-        <v>260</v>
+        <v>56</v>
       </c>
       <c r="O19" t="s">
-        <v>261</v>
+        <v>57</v>
       </c>
       <c r="P19" t="s">
         <v>263</v>
       </c>
       <c r="Q19" t="s">
-        <v>262</v>
-      </c>
-      <c r="R19" t="s">
-        <v>264</v>
+        <v>58</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="S19">
         <v>9898989898</v>
@@ -2015,8 +2027,8 @@
       <c r="I21" t="s">
         <v>309</v>
       </c>
-      <c r="X21" s="5" t="s">
-        <v>307</v>
+      <c r="X21" s="8" t="s">
+        <v>269</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>67</v>
@@ -2786,9 +2798,11 @@
     <hyperlink ref="K49" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="K50" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="B51" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="X21" r:id="rId28" display="https://mcloud-na-stage3.drybar.com/eu/baby-buttercup-travel-blow-dryer-uk" xr:uid="{C5D8E771-F17E-4B99-BE8A-605D84AEFAC1}"/>
+    <hyperlink ref="B2" r:id="rId29" xr:uid="{FB943272-A9E9-4396-B81B-EE1D123EAE70}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
reset password drybar eu
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3325A9CB-C7E2-40F1-8BC2-1C2B95E8E7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D0A6D1-83DE-4533-B079-4C8F6325063D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="331">
   <si>
     <t>UserName</t>
   </si>
@@ -1025,6 +1025,9 @@
   </si>
   <si>
     <t>DRYEUQATEST20</t>
+  </si>
+  <si>
+    <t>Flat Mate Boar Bristle Brush</t>
   </si>
 </sst>
 </file>
@@ -1459,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE32" sqref="AE32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,8 +1627,12 @@
         <v>327</v>
       </c>
       <c r="C2" s="8"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="F2" t="s">
         <v>48</v>
       </c>
@@ -1708,7 +1715,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="X6" t="s">
-        <v>269</v>
+        <v>330</v>
       </c>
       <c r="Y6" s="5">
         <v>2</v>
@@ -2828,9 +2835,11 @@
     <hyperlink ref="B51" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
     <hyperlink ref="X21" r:id="rId28" display="https://mcloud-na-stage3.drybar.com/eu/baby-buttercup-travel-blow-dryer-uk" xr:uid="{C5D8E771-F17E-4B99-BE8A-605D84AEFAC1}"/>
     <hyperlink ref="B2" r:id="rId29" xr:uid="{FB943272-A9E9-4396-B81B-EE1D123EAE70}"/>
+    <hyperlink ref="D2" r:id="rId30" xr:uid="{1E241DC1-1239-4E6B-8560-35A82A5A5295}"/>
+    <hyperlink ref="E2" r:id="rId31" xr:uid="{239D94B8-3CE6-486E-A3AE-E33383795014}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Drybar EU Commited 17 test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D0A6D1-83DE-4533-B079-4C8F6325063D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0477BDB0-578E-4006-AEC8-799EC33A1548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22560" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="331">
   <si>
     <t>UserName</t>
   </si>
@@ -724,9 +724,6 @@
   </si>
   <si>
     <t>SortBy</t>
-  </si>
-  <si>
-    <t>Highest Price</t>
   </si>
   <si>
     <t>Valid_Search</t>
@@ -1028,6 +1025,9 @@
   </si>
   <si>
     <t>Flat Mate Boar Bristle Brush</t>
+  </si>
+  <si>
+    <t>Highest price</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1571,10 +1571,10 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>96</v>
@@ -1613,7 +1613,7 @@
         <v>155</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>204</v>
@@ -1624,7 +1624,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="2" t="s">
@@ -1640,24 +1640,24 @@
         <v>47</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
+        <v>259</v>
+      </c>
+      <c r="O2" t="s">
         <v>260</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q2" t="s">
         <v>261</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>263</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>262</v>
-      </c>
-      <c r="R2" t="s">
-        <v>264</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -1665,7 +1665,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
       <c r="AK2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
@@ -1677,7 +1677,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
       <c r="AK3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
@@ -1689,7 +1689,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
       <c r="AK4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
@@ -1697,7 +1697,7 @@
         <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="4"/>
@@ -1705,7 +1705,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
       <c r="AK5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
@@ -1715,7 +1715,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="X6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Y6" s="5">
         <v>2</v>
@@ -1725,17 +1725,17 @@
         <v>4</v>
       </c>
       <c r="AK6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="X7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Y7" s="5">
         <v>2</v>
@@ -1743,7 +1743,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
       <c r="AK7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
@@ -1753,7 +1753,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="X8" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>160</v>
@@ -1761,7 +1761,7 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AK8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
@@ -1785,19 +1785,19 @@
       </c>
       <c r="L9" s="2"/>
       <c r="N9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O9" t="s">
         <v>57</v>
       </c>
       <c r="P9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="R9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>153</v>
@@ -1806,7 +1806,7 @@
         <v>165</v>
       </c>
       <c r="AK9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AK10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
@@ -1838,7 +1838,7 @@
         <v>123</v>
       </c>
       <c r="AK11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
@@ -1857,7 +1857,7 @@
         <v>123</v>
       </c>
       <c r="AK12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
@@ -1874,15 +1874,15 @@
         <v>123</v>
       </c>
       <c r="AK13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>303</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>305</v>
       </c>
       <c r="V14" s="6" t="s">
         <v>71</v>
@@ -1891,7 +1891,7 @@
         <v>123</v>
       </c>
       <c r="AK14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
@@ -1902,7 +1902,7 @@
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
       <c r="AK15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
@@ -1912,7 +1912,7 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="AK16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
@@ -1935,7 +1935,7 @@
         <v>123</v>
       </c>
       <c r="AK17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
@@ -1970,7 +1970,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.25">
@@ -1978,7 +1978,7 @@
         <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F19" t="s">
         <v>47</v>
@@ -1987,7 +1987,7 @@
         <v>48</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N19" t="s">
         <v>49</v>
@@ -2008,7 +2008,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
@@ -2016,10 +2016,10 @@
         <v>62</v>
       </c>
       <c r="H20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -2034,7 +2034,7 @@
       <c r="Z20" s="9"/>
       <c r="AA20" s="9"/>
       <c r="AK20" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
@@ -2042,13 +2042,13 @@
         <v>65</v>
       </c>
       <c r="H21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="X21" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>67</v>
@@ -2056,10 +2056,10 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
       <c r="AK21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AO21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
@@ -2094,7 +2094,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
@@ -2108,25 +2108,25 @@
         <v>79</v>
       </c>
       <c r="N23" t="s">
+        <v>269</v>
+      </c>
+      <c r="O23" t="s">
         <v>270</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q23" t="s">
         <v>271</v>
       </c>
-      <c r="P23" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q23" t="s">
+      <c r="R23" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="R23" s="5" t="s">
-        <v>273</v>
       </c>
       <c r="S23">
         <v>9898989898</v>
       </c>
       <c r="AK23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.25">
@@ -2145,22 +2145,22 @@
         <v>85</v>
       </c>
       <c r="M24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N24" t="s">
+        <v>259</v>
+      </c>
+      <c r="O24" t="s">
         <v>260</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q24" t="s">
         <v>261</v>
       </c>
-      <c r="P24" t="s">
+      <c r="R24" t="s">
         <v>263</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>262</v>
-      </c>
-      <c r="R24" t="s">
-        <v>264</v>
       </c>
       <c r="S24" s="22" t="s">
         <v>210</v>
@@ -2172,7 +2172,7 @@
       <c r="AF24" s="5"/>
       <c r="AG24" s="5"/>
       <c r="AK24" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
@@ -2180,20 +2180,20 @@
         <v>94</v>
       </c>
       <c r="X25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Y25" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z25" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AA25" s="5"/>
       <c r="AB25" s="25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AK25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
@@ -2207,7 +2207,7 @@
         <v>79</v>
       </c>
       <c r="I26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>46</v>
@@ -2231,7 +2231,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
@@ -2239,28 +2239,28 @@
         <v>104</v>
       </c>
       <c r="M27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="R27" s="10"/>
       <c r="S27" s="9"/>
       <c r="AK27" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>288</v>
+      </c>
+      <c r="M28" t="s">
         <v>289</v>
       </c>
-      <c r="M28" t="s">
-        <v>290</v>
-      </c>
       <c r="N28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
       <c r="AK28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
@@ -2268,10 +2268,10 @@
         <v>105</v>
       </c>
       <c r="M29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AK29" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
@@ -2288,7 +2288,7 @@
         <v>112</v>
       </c>
       <c r="AK30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
@@ -2299,7 +2299,7 @@
         <v>87</v>
       </c>
       <c r="AK31" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
@@ -2309,24 +2309,24 @@
         <v>145</v>
       </c>
       <c r="AE32" s="26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AF32" s="26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AK32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>301</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>327</v>
+      </c>
+      <c r="AL33" s="7" t="s">
         <v>302</v>
-      </c>
-      <c r="AK33" t="s">
-        <v>328</v>
-      </c>
-      <c r="AL33" s="7" t="s">
-        <v>303</v>
       </c>
       <c r="AM33" s="7" t="s">
         <v>157</v>
@@ -2334,13 +2334,13 @@
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>309</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>327</v>
+      </c>
+      <c r="AL34" s="7" t="s">
         <v>310</v>
-      </c>
-      <c r="AK34" t="s">
-        <v>328</v>
-      </c>
-      <c r="AL34" s="7" t="s">
-        <v>311</v>
       </c>
       <c r="AM34" s="7"/>
     </row>
@@ -2352,7 +2352,7 @@
         <v>162</v>
       </c>
       <c r="AK35" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
@@ -2368,7 +2368,7 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="5"/>
       <c r="AK36" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
@@ -2394,7 +2394,7 @@
         <v>167</v>
       </c>
       <c r="AK37" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
@@ -2413,7 +2413,7 @@
         <v>97</v>
       </c>
       <c r="AK38" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
@@ -2438,7 +2438,7 @@
         <v>178</v>
       </c>
       <c r="AK39" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
@@ -2449,10 +2449,10 @@
         <v>78</v>
       </c>
       <c r="AK40" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AL40" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AM40" s="7" t="s">
         <v>157</v>
@@ -2472,7 +2472,7 @@
         <v>182</v>
       </c>
       <c r="AK41" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
@@ -2519,7 +2519,7 @@
         <v>186</v>
       </c>
       <c r="AK42" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
         <v>168</v>
       </c>
       <c r="AK43" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.25">
@@ -2567,7 +2567,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK44" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
@@ -2601,25 +2601,25 @@
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" t="s">
+        <v>259</v>
+      </c>
+      <c r="O45" t="s">
         <v>260</v>
       </c>
-      <c r="O45" t="s">
+      <c r="P45" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q45" t="s">
         <v>261</v>
       </c>
-      <c r="P45" t="s">
+      <c r="R45" t="s">
         <v>263</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>262</v>
-      </c>
-      <c r="R45" t="s">
-        <v>264</v>
       </c>
       <c r="S45">
         <v>9898989898</v>
       </c>
       <c r="AK45" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="46" spans="1:40" x14ac:dyDescent="0.25">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="M46" s="9"/>
       <c r="AK46" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="47" spans="1:40" x14ac:dyDescent="0.25">
@@ -2663,18 +2663,18 @@
         <v>2</v>
       </c>
       <c r="AK47" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="AK48" t="s">
+        <v>327</v>
+      </c>
+      <c r="AN48" t="s">
         <v>255</v>
-      </c>
-      <c r="AK48" t="s">
-        <v>328</v>
-      </c>
-      <c r="AN48" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="49" spans="1:41" x14ac:dyDescent="0.25">
@@ -2709,57 +2709,57 @@
         <v>9898989898</v>
       </c>
       <c r="AK49" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="50" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="K50" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="K50" s="8" t="s">
+      <c r="AJ50" t="s">
         <v>280</v>
       </c>
-      <c r="AJ50" t="s">
-        <v>281</v>
-      </c>
       <c r="AK50" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>181</v>
       </c>
       <c r="X51" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Y51">
         <v>2</v>
       </c>
       <c r="AK51" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="52" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="X52" t="s">
         <v>285</v>
-      </c>
-      <c r="X52" t="s">
-        <v>286</v>
       </c>
       <c r="Y52">
         <v>2</v>
       </c>
       <c r="AK52" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H53" t="s">
         <v>62</v>
@@ -2768,7 +2768,7 @@
         <v>63</v>
       </c>
       <c r="X53" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Y53" s="5" t="s">
         <v>67</v>
@@ -2776,32 +2776,32 @@
       <c r="Z53" s="5"/>
       <c r="AA53" s="5"/>
       <c r="AK53" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AO53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>320</v>
+      </c>
+      <c r="AK54" t="s">
+        <v>327</v>
+      </c>
+      <c r="AL54" t="s">
         <v>321</v>
-      </c>
-      <c r="AK54" t="s">
-        <v>328</v>
-      </c>
-      <c r="AL54" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="55" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AK55" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AL55" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2983,22 +2983,22 @@
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q3" t="s">
         <v>97</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
       <c r="Y3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -3096,7 +3096,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>123</v>
@@ -3149,19 +3149,19 @@
         <v>79</v>
       </c>
       <c r="I2" t="s">
+        <v>259</v>
+      </c>
+      <c r="J2" t="s">
         <v>260</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L2" t="s">
         <v>261</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>263</v>
-      </c>
-      <c r="L2" t="s">
-        <v>262</v>
-      </c>
-      <c r="M2" t="s">
-        <v>264</v>
       </c>
       <c r="N2">
         <v>9898989898</v>
@@ -3183,24 +3183,24 @@
         <v>97</v>
       </c>
       <c r="V3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="W3" s="5" t="s">
         <v>67</v>
       </c>
       <c r="AB3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AB4" t="s">
+        <v>292</v>
+      </c>
+      <c r="AC4" s="8" t="s">
         <v>293</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -3281,7 +3281,7 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>22</v>
@@ -3310,7 +3310,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
@@ -3346,7 +3346,7 @@
         <v>209</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -3360,24 +3360,24 @@
         <v>79</v>
       </c>
       <c r="I3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J3" t="s">
+        <v>270</v>
+      </c>
+      <c r="K3" t="s">
         <v>271</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>273</v>
-      </c>
       <c r="M3" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>213</v>
@@ -3403,7 +3403,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G5" t="s">
         <v>78</v>
@@ -3412,24 +3412,24 @@
         <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J5" t="s">
+        <v>270</v>
+      </c>
+      <c r="K5" t="s">
         <v>271</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>273</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G6" t="s">
         <v>78</v>
@@ -3450,10 +3450,10 @@
         <v>209</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -3474,8 +3474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3653,23 +3653,23 @@
         <v>230</v>
       </c>
       <c r="AB5" t="s">
-        <v>231</v>
+        <v>330</v>
       </c>
       <c r="AC5" t="s">
-        <v>142</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="Y6" t="s">
-        <v>164</v>
-      </c>
-      <c r="Z6" s="5" t="s">
-        <v>67</v>
+        <v>268</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
@@ -3747,7 +3747,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -3759,7 +3759,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -3778,7 +3778,7 @@
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>67</v>
@@ -3787,25 +3787,25 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>164</v>
@@ -3816,13 +3816,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>164</v>
       </c>
       <c r="H7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3844,7 +3844,7 @@
         <v>65</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3895,25 +3895,25 @@
         <v>61</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>63</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>64</v>
@@ -4046,7 +4046,7 @@
         <v>175</v>
       </c>
       <c r="I3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P3" s="2"/>
       <c r="S3" s="2"/>
@@ -4064,10 +4064,10 @@
         <v>62</v>
       </c>
       <c r="H4" t="s">
+        <v>239</v>
+      </c>
+      <c r="J4" t="s">
         <v>240</v>
-      </c>
-      <c r="J4" t="s">
-        <v>241</v>
       </c>
       <c r="AF4" s="3"/>
       <c r="AG4" s="4"/>
@@ -4075,13 +4075,13 @@
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>241</v>
+      </c>
+      <c r="H5" t="s">
+        <v>239</v>
+      </c>
+      <c r="K5" t="s">
         <v>242</v>
-      </c>
-      <c r="H5" t="s">
-        <v>240</v>
-      </c>
-      <c r="K5" t="s">
-        <v>243</v>
       </c>
       <c r="AF5" s="3"/>
       <c r="AG5" s="4"/>
@@ -4089,26 +4089,26 @@
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>243</v>
+      </c>
+      <c r="H6" t="s">
         <v>244</v>
       </c>
-      <c r="H6" t="s">
+      <c r="L6" t="s">
         <v>245</v>
-      </c>
-      <c r="L6" t="s">
-        <v>246</v>
       </c>
       <c r="Z6" s="2"/>
       <c r="AM6" s="5"/>
     </row>
     <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>246</v>
+      </c>
+      <c r="H7" t="s">
         <v>247</v>
       </c>
-      <c r="H7" t="s">
+      <c r="M7" t="s">
         <v>248</v>
-      </c>
-      <c r="M7" t="s">
-        <v>249</v>
       </c>
       <c r="P7" s="7"/>
       <c r="Y7" s="7"/>
@@ -4117,10 +4117,10 @@
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>249</v>
+      </c>
+      <c r="H8" t="s">
         <v>250</v>
-      </c>
-      <c r="H8" t="s">
-        <v>251</v>
       </c>
       <c r="N8" t="s">
         <v>18</v>
@@ -4132,13 +4132,13 @@
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>251</v>
+      </c>
+      <c r="H9" t="s">
         <v>252</v>
       </c>
-      <c r="H9" t="s">
+      <c r="O9" t="s">
         <v>253</v>
-      </c>
-      <c r="O9" t="s">
-        <v>254</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Y9" s="2"/>
@@ -4469,10 +4469,10 @@
         <v>124</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>143</v>
@@ -4520,10 +4520,10 @@
         <v>131</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>143</v>
@@ -4572,10 +4572,10 @@
         <v>134</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>67</v>
@@ -4623,10 +4623,10 @@
       </c>
       <c r="H5" s="8"/>
       <c r="K5" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -4634,13 +4634,13 @@
         <v>17</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>67</v>
       </c>
       <c r="V6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="X6" s="7"/>
     </row>
@@ -4649,7 +4649,7 @@
         <v>23</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>138</v>
@@ -4817,19 +4817,19 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
+        <v>259</v>
+      </c>
+      <c r="O2" t="s">
         <v>260</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q2" t="s">
         <v>261</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>263</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>262</v>
-      </c>
-      <c r="R2" t="s">
-        <v>264</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -4851,7 +4851,7 @@
         <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="4"/>
@@ -4948,19 +4948,19 @@
         <v>46</v>
       </c>
       <c r="N10" t="s">
+        <v>259</v>
+      </c>
+      <c r="O10" t="s">
         <v>260</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q10" t="s">
         <v>261</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>263</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>262</v>
-      </c>
-      <c r="R10" t="s">
-        <v>264</v>
       </c>
       <c r="S10">
         <v>9898989898</v>
@@ -4974,7 +4974,7 @@
         <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J11" t="s">
         <v>64</v>
@@ -4992,7 +4992,7 @@
         <v>65</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>67</v>
@@ -5059,7 +5059,7 @@
         <v>94</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Y15" s="5" t="s">
         <v>67</v>
@@ -5209,7 +5209,7 @@
         <v>96</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>40</v>
@@ -5268,19 +5268,19 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
+        <v>259</v>
+      </c>
+      <c r="O2" t="s">
         <v>260</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q2" t="s">
         <v>261</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>263</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>262</v>
-      </c>
-      <c r="R2" t="s">
-        <v>264</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -5288,7 +5288,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
       <c r="AI2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -5300,7 +5300,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
       <c r="AI3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -5312,7 +5312,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
       <c r="AI4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -5320,13 +5320,13 @@
         <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="4"/>
       <c r="Y5" s="5"/>
       <c r="AI5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -5336,13 +5336,13 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="X6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Y6" s="5">
         <v>2</v>
       </c>
       <c r="AI6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -5358,7 +5358,7 @@
         <v>160</v>
       </c>
       <c r="AI7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -5371,35 +5371,35 @@
         <v>2</v>
       </c>
       <c r="AI8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="Y9" s="5"/>
       <c r="AI9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AJ9" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="Y10" s="5"/>
       <c r="AI10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AJ10" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -5416,7 +5416,7 @@
         <v>123</v>
       </c>
       <c r="AI11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -5435,7 +5435,7 @@
         <v>123</v>
       </c>
       <c r="AI12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -5452,15 +5452,15 @@
         <v>123</v>
       </c>
       <c r="AI13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>303</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>305</v>
       </c>
       <c r="V14" s="6" t="s">
         <v>71</v>
@@ -5469,7 +5469,7 @@
         <v>123</v>
       </c>
       <c r="AI14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -5479,7 +5479,7 @@
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="AI15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -5502,7 +5502,7 @@
         <v>123</v>
       </c>
       <c r="AI16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -5512,7 +5512,7 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="AI17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -5529,25 +5529,25 @@
         <v>46</v>
       </c>
       <c r="N18" t="s">
+        <v>259</v>
+      </c>
+      <c r="O18" t="s">
         <v>260</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q18" t="s">
         <v>261</v>
       </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
         <v>263</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>262</v>
-      </c>
-      <c r="R18" t="s">
-        <v>264</v>
       </c>
       <c r="S18">
         <v>9898989898</v>
       </c>
       <c r="AI18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -5582,7 +5582,7 @@
         <v>9898989898</v>
       </c>
       <c r="AI19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -5590,10 +5590,10 @@
         <v>62</v>
       </c>
       <c r="H20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -5606,7 +5606,7 @@
       <c r="X20" s="9"/>
       <c r="Y20" s="9"/>
       <c r="AI20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -5614,13 +5614,13 @@
         <v>65</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>67</v>
       </c>
       <c r="AI21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -5655,7 +5655,7 @@
         <v>9898989898</v>
       </c>
       <c r="AI22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -5687,7 +5687,7 @@
         <v>9898989898</v>
       </c>
       <c r="AI23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -5706,22 +5706,22 @@
         <v>85</v>
       </c>
       <c r="M24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N24" t="s">
+        <v>259</v>
+      </c>
+      <c r="O24" t="s">
         <v>260</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q24" t="s">
         <v>261</v>
       </c>
-      <c r="P24" t="s">
+      <c r="R24" t="s">
         <v>263</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>262</v>
-      </c>
-      <c r="R24" t="s">
-        <v>264</v>
       </c>
       <c r="S24" s="9">
         <v>9898989898</v>
@@ -5733,12 +5733,12 @@
       <c r="AD24" s="5"/>
       <c r="AE24" s="5"/>
       <c r="AI24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="7"/>
@@ -5748,10 +5748,10 @@
       <c r="H25" s="7"/>
       <c r="K25" s="2"/>
       <c r="M25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
@@ -5761,7 +5761,7 @@
       <c r="AD25" s="5"/>
       <c r="AE25" s="5"/>
       <c r="AI25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -5769,19 +5769,19 @@
         <v>94</v>
       </c>
       <c r="X26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Y26" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AA26" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AI26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -5901,7 +5901,7 @@
         <v>172</v>
       </c>
       <c r="X36" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Y36" s="5" t="s">
         <v>67</v>
@@ -5978,10 +5978,10 @@
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>322</v>
+      </c>
+      <c r="X40" s="24" t="s">
         <v>323</v>
-      </c>
-      <c r="X40" s="24" t="s">
-        <v>324</v>
       </c>
       <c r="Y40" s="5" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Drybar EU- 007 test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0477BDB0-578E-4006-AEC8-799EC33A1548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF5C2E8-6D6E-444A-8434-348E446EA7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22560" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="335">
   <si>
     <t>UserName</t>
   </si>
@@ -952,9 +952,6 @@
   </si>
   <si>
     <t>Buttercup Blow-Dryer</t>
-  </si>
-  <si>
-    <t>TEST_DRYBAR_PROMO_5759</t>
   </si>
   <si>
     <t xml:space="preserve"> All Hair Tools</t>
@@ -1028,6 +1025,21 @@
   </si>
   <si>
     <t>Highest price</t>
+  </si>
+  <si>
+    <t>Via delle Azalee 136</t>
+  </si>
+  <si>
+    <t>Belgirate</t>
+  </si>
+  <si>
+    <t>Aosta</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>TEST_DRYBAR_PROMO_3826</t>
   </si>
 </sst>
 </file>
@@ -1462,8 +1474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="AJ30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL43" sqref="AL43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,7 +1583,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>257</v>
@@ -1624,11 +1636,11 @@
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>326</v>
+        <v>188</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="2" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>60</v>
@@ -1640,24 +1652,24 @@
         <v>47</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
-        <v>259</v>
+        <v>330</v>
       </c>
       <c r="O2" t="s">
-        <v>260</v>
+        <v>331</v>
       </c>
       <c r="P2" t="s">
-        <v>262</v>
+        <v>333</v>
       </c>
       <c r="Q2" t="s">
-        <v>261</v>
-      </c>
-      <c r="R2" t="s">
-        <v>263</v>
+        <v>332</v>
+      </c>
+      <c r="R2">
+        <v>28832</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -1665,7 +1677,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
       <c r="AK2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
@@ -1677,7 +1689,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
       <c r="AK3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
@@ -1689,7 +1701,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
       <c r="AK4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
@@ -1705,7 +1717,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
       <c r="AK5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
@@ -1715,7 +1727,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="X6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Y6" s="5">
         <v>2</v>
@@ -1725,7 +1737,7 @@
         <v>4</v>
       </c>
       <c r="AK6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
@@ -1743,7 +1755,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
       <c r="AK7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
@@ -1753,7 +1765,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="X8" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>160</v>
@@ -1761,7 +1773,7 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AK8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
@@ -1806,7 +1818,7 @@
         <v>165</v>
       </c>
       <c r="AK9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
@@ -1821,7 +1833,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AK10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
@@ -1838,7 +1850,7 @@
         <v>123</v>
       </c>
       <c r="AK11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
@@ -1857,7 +1869,7 @@
         <v>123</v>
       </c>
       <c r="AK12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
@@ -1874,7 +1886,7 @@
         <v>123</v>
       </c>
       <c r="AK13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
@@ -1891,7 +1903,7 @@
         <v>123</v>
       </c>
       <c r="AK14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
@@ -1902,7 +1914,7 @@
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
       <c r="AK15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
@@ -1912,7 +1924,7 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="AK16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
@@ -1935,7 +1947,7 @@
         <v>123</v>
       </c>
       <c r="AK17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
@@ -1970,7 +1982,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.25">
@@ -1978,7 +1990,7 @@
         <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F19" t="s">
         <v>47</v>
@@ -1987,7 +1999,7 @@
         <v>48</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N19" t="s">
         <v>49</v>
@@ -2008,7 +2020,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
@@ -2019,7 +2031,7 @@
         <v>239</v>
       </c>
       <c r="I20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -2034,7 +2046,7 @@
       <c r="Z20" s="9"/>
       <c r="AA20" s="9"/>
       <c r="AK20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
@@ -2045,7 +2057,7 @@
         <v>239</v>
       </c>
       <c r="I21" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="X21" s="8" t="s">
         <v>268</v>
@@ -2056,7 +2068,7 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
       <c r="AK21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AO21" t="s">
         <v>286</v>
@@ -2094,7 +2106,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK22" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
@@ -2126,7 +2138,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.25">
@@ -2172,7 +2184,7 @@
       <c r="AF24" s="5"/>
       <c r="AG24" s="5"/>
       <c r="AK24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
@@ -2180,20 +2192,20 @@
         <v>94</v>
       </c>
       <c r="X25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Y25" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z25" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AA25" s="5"/>
       <c r="AB25" s="25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AK25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
@@ -2231,7 +2243,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK26" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
@@ -2244,7 +2256,7 @@
       <c r="R27" s="10"/>
       <c r="S27" s="9"/>
       <c r="AK27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
@@ -2260,7 +2272,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
       <c r="AK28" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
@@ -2271,7 +2283,7 @@
         <v>289</v>
       </c>
       <c r="AK29" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
@@ -2288,7 +2300,7 @@
         <v>112</v>
       </c>
       <c r="AK30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
@@ -2299,7 +2311,7 @@
         <v>87</v>
       </c>
       <c r="AK31" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
@@ -2309,13 +2321,13 @@
         <v>145</v>
       </c>
       <c r="AE32" s="26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF32" s="26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AK32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
@@ -2323,7 +2335,7 @@
         <v>301</v>
       </c>
       <c r="AK33" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AL33" s="7" t="s">
         <v>302</v>
@@ -2334,13 +2346,13 @@
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>308</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>326</v>
+      </c>
+      <c r="AL34" s="7" t="s">
         <v>309</v>
-      </c>
-      <c r="AK34" t="s">
-        <v>327</v>
-      </c>
-      <c r="AL34" s="7" t="s">
-        <v>310</v>
       </c>
       <c r="AM34" s="7"/>
     </row>
@@ -2352,7 +2364,7 @@
         <v>162</v>
       </c>
       <c r="AK35" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
@@ -2368,7 +2380,7 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="5"/>
       <c r="AK36" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
@@ -2394,7 +2406,7 @@
         <v>167</v>
       </c>
       <c r="AK37" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
@@ -2413,7 +2425,7 @@
         <v>97</v>
       </c>
       <c r="AK38" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
@@ -2438,7 +2450,7 @@
         <v>178</v>
       </c>
       <c r="AK39" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
@@ -2449,10 +2461,10 @@
         <v>78</v>
       </c>
       <c r="AK40" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AL40" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
       <c r="AM40" s="7" t="s">
         <v>157</v>
@@ -2472,7 +2484,7 @@
         <v>182</v>
       </c>
       <c r="AK41" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
@@ -2519,7 +2531,7 @@
         <v>186</v>
       </c>
       <c r="AK42" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
@@ -2535,7 +2547,7 @@
         <v>168</v>
       </c>
       <c r="AK43" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.25">
@@ -2567,7 +2579,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK44" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
@@ -2619,7 +2631,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK45" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="46" spans="1:40" x14ac:dyDescent="0.25">
@@ -2649,7 +2661,7 @@
       </c>
       <c r="M46" s="9"/>
       <c r="AK46" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="47" spans="1:40" x14ac:dyDescent="0.25">
@@ -2663,7 +2675,7 @@
         <v>2</v>
       </c>
       <c r="AK47" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.25">
@@ -2671,7 +2683,7 @@
         <v>254</v>
       </c>
       <c r="AK48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AN48" t="s">
         <v>255</v>
@@ -2709,7 +2721,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="50" spans="1:41" x14ac:dyDescent="0.25">
@@ -2723,7 +2735,7 @@
         <v>280</v>
       </c>
       <c r="AK50" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.25">
@@ -2740,7 +2752,7 @@
         <v>2</v>
       </c>
       <c r="AK51" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="52" spans="1:41" x14ac:dyDescent="0.25">
@@ -2754,7 +2766,7 @@
         <v>2</v>
       </c>
       <c r="AK52" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.25">
@@ -2776,7 +2788,7 @@
       <c r="Z53" s="5"/>
       <c r="AA53" s="5"/>
       <c r="AK53" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AO53" t="s">
         <v>286</v>
@@ -2784,21 +2796,21 @@
     </row>
     <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>319</v>
+      </c>
+      <c r="AK54" t="s">
+        <v>326</v>
+      </c>
+      <c r="AL54" t="s">
         <v>320</v>
-      </c>
-      <c r="AK54" t="s">
-        <v>327</v>
-      </c>
-      <c r="AL54" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="55" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AK55" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AL55" s="7" t="s">
         <v>302</v>
@@ -2983,16 +2995,16 @@
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q3" t="s">
         <v>97</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -3453,7 +3465,7 @@
         <v>296</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -3474,7 +3486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView topLeftCell="V1" workbookViewId="0">
       <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
@@ -3653,10 +3665,10 @@
         <v>230</v>
       </c>
       <c r="AB5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AC5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -4974,7 +4986,7 @@
         <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J11" t="s">
         <v>64</v>
@@ -5209,7 +5221,7 @@
         <v>96</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>40</v>
@@ -5390,7 +5402,7 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -5399,7 +5411,7 @@
         <v>258</v>
       </c>
       <c r="AJ10" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -5593,7 +5605,7 @@
         <v>239</v>
       </c>
       <c r="I20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -5769,16 +5781,16 @@
         <v>94</v>
       </c>
       <c r="X26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Y26" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AA26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AI26" t="s">
         <v>258</v>
@@ -5901,7 +5913,7 @@
         <v>172</v>
       </c>
       <c r="X36" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Y36" s="5" t="s">
         <v>67</v>
@@ -5978,10 +5990,10 @@
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>321</v>
+      </c>
+      <c r="X40" s="24" t="s">
         <v>322</v>
-      </c>
-      <c r="X40" s="24" t="s">
-        <v>323</v>
       </c>
       <c r="Y40" s="5" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
DRY EU 11, 16 testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF5C2E8-6D6E-444A-8434-348E446EA7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25273FE-CF0F-4803-BFA7-9F47A50BBC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="340">
   <si>
     <t>UserName</t>
   </si>
@@ -1012,9 +1012,6 @@
 T: 9999999999</t>
   </si>
   <si>
-    <t>vnarra@helenoftroy.com</t>
-  </si>
-  <si>
     <t>€</t>
   </si>
   <si>
@@ -1040,6 +1037,24 @@
   </si>
   <si>
     <t>TEST_DRYBAR_PROMO_3826</t>
+  </si>
+  <si>
+    <t>skasarla@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Brandenburgische Str. 58</t>
+  </si>
+  <si>
+    <t>Hennigsdorf</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>16761</t>
   </si>
 </sst>
 </file>
@@ -1474,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL43" sqref="AL43"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,13 +1650,9 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>188</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="2" t="s">
-        <v>168</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
         <v>60</v>
       </c>
@@ -1651,22 +1662,20 @@
       <c r="G2" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>325</v>
-      </c>
+      <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
+        <v>329</v>
+      </c>
+      <c r="O2" t="s">
         <v>330</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q2" t="s">
         <v>331</v>
-      </c>
-      <c r="P2" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>332</v>
       </c>
       <c r="R2">
         <v>28832</v>
@@ -1677,7 +1686,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
       <c r="AK2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
@@ -1689,7 +1698,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
       <c r="AK3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
@@ -1701,7 +1710,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
       <c r="AK4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
@@ -1717,7 +1726,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
       <c r="AK5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
@@ -1727,7 +1736,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="X6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Y6" s="5">
         <v>2</v>
@@ -1737,7 +1746,7 @@
         <v>4</v>
       </c>
       <c r="AK6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
@@ -1755,7 +1764,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
       <c r="AK7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
@@ -1773,7 +1782,7 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AK8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
@@ -1818,7 +1827,7 @@
         <v>165</v>
       </c>
       <c r="AK9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
@@ -1833,7 +1842,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AK10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
@@ -1850,7 +1859,7 @@
         <v>123</v>
       </c>
       <c r="AK11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
@@ -1869,7 +1878,7 @@
         <v>123</v>
       </c>
       <c r="AK12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
@@ -1886,7 +1895,7 @@
         <v>123</v>
       </c>
       <c r="AK13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
@@ -1903,7 +1912,7 @@
         <v>123</v>
       </c>
       <c r="AK14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
@@ -1914,7 +1923,7 @@
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
       <c r="AK15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
@@ -1924,7 +1933,7 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="AK16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
@@ -1947,7 +1956,7 @@
         <v>123</v>
       </c>
       <c r="AK17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
@@ -1982,15 +1991,15 @@
         <v>9898989898</v>
       </c>
       <c r="AK18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
-      <c r="B19" t="s">
-        <v>325</v>
+      <c r="B19" s="8" t="s">
+        <v>334</v>
       </c>
       <c r="F19" t="s">
         <v>47</v>
@@ -1999,28 +2008,28 @@
         <v>48</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="N19" t="s">
-        <v>49</v>
+        <v>335</v>
       </c>
       <c r="O19" t="s">
-        <v>50</v>
+        <v>336</v>
       </c>
       <c r="P19" t="s">
-        <v>52</v>
+        <v>337</v>
       </c>
       <c r="Q19" t="s">
-        <v>51</v>
-      </c>
-      <c r="R19">
-        <v>81504</v>
+        <v>338</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>339</v>
       </c>
       <c r="S19">
         <v>9898989898</v>
       </c>
       <c r="AK19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
@@ -2046,7 +2055,7 @@
       <c r="Z20" s="9"/>
       <c r="AA20" s="9"/>
       <c r="AK20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
@@ -2068,7 +2077,7 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
       <c r="AK21" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AO21" t="s">
         <v>286</v>
@@ -2106,7 +2115,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
@@ -2138,7 +2147,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.25">
@@ -2184,7 +2193,7 @@
       <c r="AF24" s="5"/>
       <c r="AG24" s="5"/>
       <c r="AK24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
@@ -2205,7 +2214,7 @@
         <v>318</v>
       </c>
       <c r="AK25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
@@ -2243,7 +2252,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
@@ -2256,7 +2265,7 @@
       <c r="R27" s="10"/>
       <c r="S27" s="9"/>
       <c r="AK27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
@@ -2272,7 +2281,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
       <c r="AK28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
@@ -2283,7 +2292,7 @@
         <v>289</v>
       </c>
       <c r="AK29" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
@@ -2300,7 +2309,7 @@
         <v>112</v>
       </c>
       <c r="AK30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
@@ -2311,7 +2320,7 @@
         <v>87</v>
       </c>
       <c r="AK31" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
@@ -2321,13 +2330,13 @@
         <v>145</v>
       </c>
       <c r="AE32" s="26" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AF32" s="26" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AK32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
@@ -2335,7 +2344,7 @@
         <v>301</v>
       </c>
       <c r="AK33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL33" s="7" t="s">
         <v>302</v>
@@ -2349,7 +2358,7 @@
         <v>308</v>
       </c>
       <c r="AK34" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL34" s="7" t="s">
         <v>309</v>
@@ -2364,7 +2373,7 @@
         <v>162</v>
       </c>
       <c r="AK35" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
@@ -2380,7 +2389,7 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="5"/>
       <c r="AK36" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
@@ -2406,7 +2415,7 @@
         <v>167</v>
       </c>
       <c r="AK37" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
@@ -2425,7 +2434,7 @@
         <v>97</v>
       </c>
       <c r="AK38" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
@@ -2450,7 +2459,7 @@
         <v>178</v>
       </c>
       <c r="AK39" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
@@ -2461,10 +2470,10 @@
         <v>78</v>
       </c>
       <c r="AK40" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL40" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AM40" s="7" t="s">
         <v>157</v>
@@ -2484,7 +2493,7 @@
         <v>182</v>
       </c>
       <c r="AK41" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
@@ -2531,7 +2540,7 @@
         <v>186</v>
       </c>
       <c r="AK42" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
@@ -2547,7 +2556,7 @@
         <v>168</v>
       </c>
       <c r="AK43" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.25">
@@ -2579,7 +2588,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK44" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
@@ -2631,7 +2640,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK45" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="46" spans="1:40" x14ac:dyDescent="0.25">
@@ -2661,7 +2670,7 @@
       </c>
       <c r="M46" s="9"/>
       <c r="AK46" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:40" x14ac:dyDescent="0.25">
@@ -2675,7 +2684,7 @@
         <v>2</v>
       </c>
       <c r="AK47" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.25">
@@ -2683,7 +2692,7 @@
         <v>254</v>
       </c>
       <c r="AK48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AN48" t="s">
         <v>255</v>
@@ -2721,7 +2730,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK49" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="50" spans="1:41" x14ac:dyDescent="0.25">
@@ -2735,7 +2744,7 @@
         <v>280</v>
       </c>
       <c r="AK50" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.25">
@@ -2752,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="AK51" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="52" spans="1:41" x14ac:dyDescent="0.25">
@@ -2766,7 +2775,7 @@
         <v>2</v>
       </c>
       <c r="AK52" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.25">
@@ -2788,7 +2797,7 @@
       <c r="Z53" s="5"/>
       <c r="AA53" s="5"/>
       <c r="AK53" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AO53" t="s">
         <v>286</v>
@@ -2799,7 +2808,7 @@
         <v>319</v>
       </c>
       <c r="AK54" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL54" t="s">
         <v>320</v>
@@ -2810,7 +2819,7 @@
         <v>323</v>
       </c>
       <c r="AK55" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL55" s="7" t="s">
         <v>302</v>
@@ -2846,9 +2855,9 @@
     <hyperlink ref="K50" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="B51" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
     <hyperlink ref="X21" r:id="rId28" display="https://mcloud-na-stage3.drybar.com/eu/baby-buttercup-travel-blow-dryer-uk" xr:uid="{C5D8E771-F17E-4B99-BE8A-605D84AEFAC1}"/>
-    <hyperlink ref="B2" r:id="rId29" xr:uid="{FB943272-A9E9-4396-B81B-EE1D123EAE70}"/>
-    <hyperlink ref="D2" r:id="rId30" xr:uid="{1E241DC1-1239-4E6B-8560-35A82A5A5295}"/>
-    <hyperlink ref="E2" r:id="rId31" xr:uid="{239D94B8-3CE6-486E-A3AE-E33383795014}"/>
+    <hyperlink ref="E2" r:id="rId29" xr:uid="{239D94B8-3CE6-486E-A3AE-E33383795014}"/>
+    <hyperlink ref="B19" r:id="rId30" xr:uid="{1CFDF9CA-1C69-4672-93B7-E3CE922F1535}"/>
+    <hyperlink ref="K19" r:id="rId31" xr:uid="{D93DA7CB-BB57-4B34-A75D-2F8FB71C9DE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId32"/>
@@ -3665,10 +3674,10 @@
         <v>230</v>
       </c>
       <c r="AB5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AC5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -4691,12 +4700,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4813,9 +4826,7 @@
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
         <v>60</v>
       </c>
@@ -4825,7 +4836,7 @@
       <c r="G2" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="8"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
@@ -5004,7 +5015,7 @@
         <v>65</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>306</v>
+        <v>268</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>67</v>
@@ -5021,19 +5032,19 @@
         <v>79</v>
       </c>
       <c r="N13" t="s">
-        <v>206</v>
+        <v>335</v>
       </c>
       <c r="O13" t="s">
-        <v>207</v>
+        <v>336</v>
       </c>
       <c r="P13" t="s">
-        <v>52</v>
+        <v>337</v>
       </c>
       <c r="Q13" t="s">
-        <v>208</v>
+        <v>338</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>209</v>
+        <v>339</v>
       </c>
       <c r="S13">
         <v>9898989898</v>
@@ -5110,10 +5121,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="K14" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="K10" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="K14" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="K10" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
DRY EU 13 testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25273FE-CF0F-4803-BFA7-9F47A50BBC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30979318-7267-43AD-BA3C-53B2FDE335EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="336">
   <si>
     <t>UserName</t>
   </si>
@@ -838,9 +838,6 @@
   </si>
   <si>
     <t>Baby Buttercup Travel Blow-Dryer</t>
-  </si>
-  <si>
-    <t>8 Sillerton House</t>
   </si>
   <si>
     <t>Aberdeen</t>
@@ -1024,18 +1021,6 @@
     <t>Highest price</t>
   </si>
   <si>
-    <t>Via delle Azalee 136</t>
-  </si>
-  <si>
-    <t>Belgirate</t>
-  </si>
-  <si>
-    <t>Aosta</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
     <t>TEST_DRYBAR_PROMO_3826</t>
   </si>
   <si>
@@ -1055,6 +1040,9 @@
   </si>
   <si>
     <t>16761</t>
+  </si>
+  <si>
+    <t>TEST_DRYBAR_PROMO_5969</t>
   </si>
 </sst>
 </file>
@@ -1489,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1586,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>257</v>
@@ -1666,19 +1654,19 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="O2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="P2" t="s">
         <v>332</v>
       </c>
       <c r="Q2" t="s">
-        <v>331</v>
-      </c>
-      <c r="R2">
-        <v>28832</v>
+        <v>333</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>334</v>
       </c>
       <c r="S2">
         <v>9898989898</v>
@@ -1686,7 +1674,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
       <c r="AK2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
@@ -1698,7 +1686,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="6"/>
       <c r="AK3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
@@ -1710,7 +1698,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="6"/>
       <c r="AK4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
@@ -1726,7 +1714,7 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
       <c r="AK5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
@@ -1736,7 +1724,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="X6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Y6" s="5">
         <v>2</v>
@@ -1746,17 +1734,17 @@
         <v>4</v>
       </c>
       <c r="AK6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="X7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Y7" s="5">
         <v>2</v>
@@ -1764,7 +1752,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
       <c r="AK7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
@@ -1774,7 +1762,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="X8" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>160</v>
@@ -1782,7 +1770,7 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AK8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
@@ -1827,7 +1815,7 @@
         <v>165</v>
       </c>
       <c r="AK9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
@@ -1842,7 +1830,7 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AK10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
@@ -1859,7 +1847,7 @@
         <v>123</v>
       </c>
       <c r="AK11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
@@ -1878,7 +1866,7 @@
         <v>123</v>
       </c>
       <c r="AK12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
@@ -1895,15 +1883,15 @@
         <v>123</v>
       </c>
       <c r="AK13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>302</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>303</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>304</v>
       </c>
       <c r="V14" s="6" t="s">
         <v>71</v>
@@ -1912,7 +1900,7 @@
         <v>123</v>
       </c>
       <c r="AK14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
@@ -1923,7 +1911,7 @@
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
       <c r="AK15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
@@ -1933,7 +1921,7 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="AK16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
@@ -1956,7 +1944,7 @@
         <v>123</v>
       </c>
       <c r="AK17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
@@ -1991,7 +1979,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK18" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.25">
@@ -1999,7 +1987,7 @@
         <v>55</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F19" t="s">
         <v>47</v>
@@ -2008,28 +1996,28 @@
         <v>48</v>
       </c>
       <c r="K19" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="N19" t="s">
+        <v>330</v>
+      </c>
+      <c r="O19" t="s">
+        <v>331</v>
+      </c>
+      <c r="P19" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>333</v>
+      </c>
+      <c r="R19" s="5" t="s">
         <v>334</v>
-      </c>
-      <c r="N19" t="s">
-        <v>335</v>
-      </c>
-      <c r="O19" t="s">
-        <v>336</v>
-      </c>
-      <c r="P19" t="s">
-        <v>337</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>338</v>
-      </c>
-      <c r="R19" s="5" t="s">
-        <v>339</v>
       </c>
       <c r="S19">
         <v>9898989898</v>
       </c>
       <c r="AK19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
@@ -2040,7 +2028,7 @@
         <v>239</v>
       </c>
       <c r="I20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -2055,7 +2043,7 @@
       <c r="Z20" s="9"/>
       <c r="AA20" s="9"/>
       <c r="AK20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
@@ -2066,7 +2054,7 @@
         <v>239</v>
       </c>
       <c r="I21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="X21" s="8" t="s">
         <v>268</v>
@@ -2077,10 +2065,10 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
       <c r="AK21" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AO21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
@@ -2097,25 +2085,25 @@
         <v>46</v>
       </c>
       <c r="N22" t="s">
-        <v>73</v>
+        <v>330</v>
       </c>
       <c r="O22" t="s">
-        <v>74</v>
+        <v>331</v>
       </c>
       <c r="P22" t="s">
-        <v>52</v>
+        <v>332</v>
       </c>
       <c r="Q22" t="s">
-        <v>75</v>
+        <v>333</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>76</v>
+        <v>334</v>
       </c>
       <c r="S22">
         <v>9898989898</v>
       </c>
       <c r="AK22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
@@ -2129,25 +2117,25 @@
         <v>79</v>
       </c>
       <c r="N23" t="s">
-        <v>269</v>
+        <v>330</v>
       </c>
       <c r="O23" t="s">
-        <v>270</v>
+        <v>331</v>
       </c>
       <c r="P23" t="s">
-        <v>262</v>
+        <v>332</v>
       </c>
       <c r="Q23" t="s">
-        <v>271</v>
+        <v>333</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>272</v>
+        <v>334</v>
       </c>
       <c r="S23">
         <v>9898989898</v>
       </c>
       <c r="AK23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.25">
@@ -2166,22 +2154,22 @@
         <v>85</v>
       </c>
       <c r="M24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N24" t="s">
-        <v>259</v>
+        <v>330</v>
       </c>
       <c r="O24" t="s">
-        <v>260</v>
+        <v>331</v>
       </c>
       <c r="P24" t="s">
-        <v>262</v>
+        <v>332</v>
       </c>
       <c r="Q24" t="s">
-        <v>261</v>
-      </c>
-      <c r="R24" t="s">
-        <v>263</v>
+        <v>333</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>334</v>
       </c>
       <c r="S24" s="22" t="s">
         <v>210</v>
@@ -2193,7 +2181,7 @@
       <c r="AF24" s="5"/>
       <c r="AG24" s="5"/>
       <c r="AK24" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
@@ -2201,20 +2189,20 @@
         <v>94</v>
       </c>
       <c r="X25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Y25" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z25" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AA25" s="5"/>
       <c r="AB25" s="25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AK25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
@@ -2228,7 +2216,7 @@
         <v>79</v>
       </c>
       <c r="I26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>46</v>
@@ -2252,7 +2240,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
@@ -2265,23 +2253,23 @@
       <c r="R27" s="10"/>
       <c r="S27" s="9"/>
       <c r="AK27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>287</v>
+      </c>
+      <c r="M28" t="s">
         <v>288</v>
       </c>
-      <c r="M28" t="s">
-        <v>289</v>
-      </c>
       <c r="N28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R28" s="10"/>
       <c r="S28" s="9"/>
       <c r="AK28" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
@@ -2289,10 +2277,10 @@
         <v>105</v>
       </c>
       <c r="M29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AK29" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
@@ -2309,7 +2297,7 @@
         <v>112</v>
       </c>
       <c r="AK30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
@@ -2320,7 +2308,7 @@
         <v>87</v>
       </c>
       <c r="AK31" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
@@ -2330,24 +2318,24 @@
         <v>145</v>
       </c>
       <c r="AE32" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AF32" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AK33" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AL33" s="7" t="s">
-        <v>302</v>
+        <v>335</v>
       </c>
       <c r="AM33" s="7" t="s">
         <v>157</v>
@@ -2355,13 +2343,13 @@
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>307</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>324</v>
+      </c>
+      <c r="AL34" s="7" t="s">
         <v>308</v>
-      </c>
-      <c r="AK34" t="s">
-        <v>325</v>
-      </c>
-      <c r="AL34" s="7" t="s">
-        <v>309</v>
       </c>
       <c r="AM34" s="7"/>
     </row>
@@ -2373,7 +2361,7 @@
         <v>162</v>
       </c>
       <c r="AK35" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
@@ -2389,7 +2377,7 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="5"/>
       <c r="AK36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
@@ -2415,7 +2403,7 @@
         <v>167</v>
       </c>
       <c r="AK37" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
@@ -2434,7 +2422,7 @@
         <v>97</v>
       </c>
       <c r="AK38" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
@@ -2459,7 +2447,7 @@
         <v>178</v>
       </c>
       <c r="AK39" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
@@ -2470,10 +2458,10 @@
         <v>78</v>
       </c>
       <c r="AK40" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AL40" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="AM40" s="7" t="s">
         <v>157</v>
@@ -2493,7 +2481,7 @@
         <v>182</v>
       </c>
       <c r="AK41" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
@@ -2540,7 +2528,7 @@
         <v>186</v>
       </c>
       <c r="AK42" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
@@ -2556,7 +2544,7 @@
         <v>168</v>
       </c>
       <c r="AK43" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.25">
@@ -2588,7 +2576,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK44" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
@@ -2640,7 +2628,7 @@
         <v>9898989898</v>
       </c>
       <c r="AK45" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="46" spans="1:40" x14ac:dyDescent="0.25">
@@ -2670,7 +2658,7 @@
       </c>
       <c r="M46" s="9"/>
       <c r="AK46" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="47" spans="1:40" x14ac:dyDescent="0.25">
@@ -2684,7 +2672,7 @@
         <v>2</v>
       </c>
       <c r="AK47" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.25">
@@ -2692,7 +2680,7 @@
         <v>254</v>
       </c>
       <c r="AK48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AN48" t="s">
         <v>255</v>
@@ -2730,57 +2718,57 @@
         <v>9898989898</v>
       </c>
       <c r="AK49" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="50" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="K50" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="K50" s="8" t="s">
+      <c r="AJ50" t="s">
         <v>279</v>
       </c>
-      <c r="AJ50" t="s">
-        <v>280</v>
-      </c>
       <c r="AK50" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>181</v>
       </c>
       <c r="X51" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Y51">
         <v>2</v>
       </c>
       <c r="AK51" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="52" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="X52" t="s">
         <v>284</v>
-      </c>
-      <c r="X52" t="s">
-        <v>285</v>
       </c>
       <c r="Y52">
         <v>2</v>
       </c>
       <c r="AK52" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H53" t="s">
         <v>62</v>
@@ -2789,7 +2777,7 @@
         <v>63</v>
       </c>
       <c r="X53" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Y53" s="5" t="s">
         <v>67</v>
@@ -2797,32 +2785,32 @@
       <c r="Z53" s="5"/>
       <c r="AA53" s="5"/>
       <c r="AK53" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AO53" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>318</v>
+      </c>
+      <c r="AK54" t="s">
+        <v>324</v>
+      </c>
+      <c r="AL54" t="s">
         <v>319</v>
-      </c>
-      <c r="AK54" t="s">
-        <v>325</v>
-      </c>
-      <c r="AL54" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AK55" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AL55" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -3004,16 +2992,16 @@
         <v>46</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q3" t="s">
         <v>97</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -3117,7 +3105,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>123</v>
@@ -3204,24 +3192,24 @@
         <v>97</v>
       </c>
       <c r="V3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="W3" s="5" t="s">
         <v>67</v>
       </c>
       <c r="AB3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AB4" t="s">
+        <v>291</v>
+      </c>
+      <c r="AC4" s="8" t="s">
         <v>292</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -3302,7 +3290,7 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>22</v>
@@ -3331,7 +3319,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
@@ -3367,7 +3355,7 @@
         <v>209</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -3381,24 +3369,24 @@
         <v>79</v>
       </c>
       <c r="I3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J3" t="s">
+        <v>269</v>
+      </c>
+      <c r="K3" t="s">
         <v>270</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>272</v>
-      </c>
       <c r="M3" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>213</v>
@@ -3424,7 +3412,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G5" t="s">
         <v>78</v>
@@ -3433,24 +3421,24 @@
         <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J5" t="s">
+        <v>269</v>
+      </c>
+      <c r="K5" t="s">
         <v>270</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>272</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="195" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G6" t="s">
         <v>78</v>
@@ -3471,10 +3459,10 @@
         <v>209</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -3674,10 +3662,10 @@
         <v>230</v>
       </c>
       <c r="AB5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AC5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -3768,7 +3756,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -3780,7 +3768,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -3808,12 +3796,12 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="18" t="s">
@@ -3821,7 +3809,7 @@
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3837,13 +3825,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>164</v>
       </c>
       <c r="H7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -4700,7 +4688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -4997,7 +4985,7 @@
         <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J11" t="s">
         <v>64</v>
@@ -5032,19 +5020,19 @@
         <v>79</v>
       </c>
       <c r="N13" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="O13" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="P13" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="Q13" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="S13">
         <v>9898989898</v>
@@ -5082,7 +5070,7 @@
         <v>94</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Y15" s="5" t="s">
         <v>67</v>
@@ -5231,7 +5219,7 @@
         <v>96</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>40</v>
@@ -5398,7 +5386,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -5407,12 +5395,12 @@
         <v>258</v>
       </c>
       <c r="AJ9" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -5421,7 +5409,7 @@
         <v>258</v>
       </c>
       <c r="AJ10" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -5479,10 +5467,10 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>302</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>303</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>304</v>
       </c>
       <c r="V14" s="6" t="s">
         <v>71</v>
@@ -5615,7 +5603,7 @@
         <v>239</v>
       </c>
       <c r="I20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -5636,7 +5624,7 @@
         <v>65</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Y21" s="5" t="s">
         <v>67</v>
@@ -5728,7 +5716,7 @@
         <v>85</v>
       </c>
       <c r="M24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N24" t="s">
         <v>259</v>
@@ -5760,7 +5748,7 @@
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="7"/>
@@ -5770,10 +5758,10 @@
       <c r="H25" s="7"/>
       <c r="K25" s="2"/>
       <c r="M25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
@@ -5791,16 +5779,16 @@
         <v>94</v>
       </c>
       <c r="X26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Y26" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AA26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AI26" t="s">
         <v>258</v>
@@ -5923,7 +5911,7 @@
         <v>172</v>
       </c>
       <c r="X36" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Y36" s="5" t="s">
         <v>67</v>
@@ -6000,10 +5988,10 @@
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>320</v>
+      </c>
+      <c r="X40" s="24" t="s">
         <v>321</v>
-      </c>
-      <c r="X40" s="24" t="s">
-        <v>322</v>
       </c>
       <c r="Y40" s="5" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
DRY EU 003 Testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
+++ b/src/test/resources/TestData/Drybar_EU/GoldDrybarEUTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30979318-7267-43AD-BA3C-53B2FDE335EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF22FA10-CA02-473C-A975-615ED616A73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1477,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,7 +2349,7 @@
         <v>324</v>
       </c>
       <c r="AL34" s="7" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="AM34" s="7"/>
     </row>
@@ -5121,7 +5121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AK40"/>
   <sheetViews>
-    <sheetView topLeftCell="K29" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X47" sqref="X47"/>
     </sheetView>
   </sheetViews>

</xml_diff>